<commit_message>
.PNG not .png, matters on server
</commit_message>
<xml_diff>
--- a/GeneticProgrammingPortfolio/sheets/lagged-variables-working.xlsx
+++ b/GeneticProgrammingPortfolio/sheets/lagged-variables-working.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\GitHub\GPP\GeneticProgrammingPortfolio\sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesEarle\Documents\Development\GitHub\GPP\GeneticProgrammingPortfolio\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -151,6 +151,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1071,7 +1072,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-412E-4860-9393-585A3A5755B0}"/>
             </c:ext>
@@ -1860,7 +1861,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-412E-4860-9393-585A3A5755B0}"/>
             </c:ext>
@@ -1989,7 +1990,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-412E-4860-9393-585A3A5755B0}"/>
             </c:ext>
@@ -2004,11 +2005,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="645041472"/>
-        <c:axId val="645037536"/>
+        <c:axId val="-1119346352"/>
+        <c:axId val="-1119342544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="645041472"/>
+        <c:axId val="-1119346352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2051,7 +2052,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="645037536"/>
+        <c:crossAx val="-1119342544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2059,7 +2060,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="645037536"/>
+        <c:axId val="-1119342544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2110,7 +2111,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="645041472"/>
+        <c:crossAx val="-1119346352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2124,6 +2125,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2191,7 +2193,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2230,6 +2232,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3150,7 +3153,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-C7B6-4EE3-9DF6-E17532E6E401}"/>
             </c:ext>
@@ -3939,7 +3942,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-C7B6-4EE3-9DF6-E17532E6E401}"/>
             </c:ext>
@@ -4068,7 +4071,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-C7B6-4EE3-9DF6-E17532E6E401}"/>
             </c:ext>
@@ -4083,11 +4086,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="525906224"/>
-        <c:axId val="525902616"/>
+        <c:axId val="-1284156032"/>
+        <c:axId val="-1284252480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="525906224"/>
+        <c:axId val="-1284156032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4129,7 +4132,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="525902616"/>
+        <c:crossAx val="-1284252480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4137,7 +4140,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="525902616"/>
+        <c:axId val="-1284252480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4188,7 +4191,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="525906224"/>
+        <c:crossAx val="-1284156032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4202,6 +4205,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5385,15 +5389,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54908</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>574453</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>34636</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5414,14 +5418,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>11765</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>531310</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>246783</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>35299</xdr:rowOff>
     </xdr:to>
@@ -8864,7 +8868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="T33" sqref="T33"/>
     </sheetView>
   </sheetViews>

</xml_diff>